<commit_message>
Corrected pharmacy type binding in Org
Corrected pharmacy type binding in pharmacy Organization resourcce profile
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-pharmacy-Organization.xlsx
+++ b/output/carin-rtpbc-pharmacy-Organization.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="437">
   <si>
     <t>Path</t>
   </si>
@@ -623,7 +623,7 @@
   </si>
   <si>
     <t>&lt;valueIdentifier xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="http://example.org/ncpdpid/placeholder"/&gt;
+  &lt;system value="http://ncpdp.org/provider-id"/&gt;
 &lt;/valueIdentifier&gt;</t>
   </si>
   <si>
@@ -665,10 +665,10 @@
     <t>Organization.type</t>
   </si>
   <si>
-    <t>Kind of organization</t>
-  </si>
-  <si>
-    <t>The kind(s) of organization that this is.</t>
+    <t>Pharmacy Type</t>
+  </si>
+  <si>
+    <t>Pharmacy type: R (Retail), M (Mail order), S (Specialty), L (Long-term care), A (Pharmacy without restriction)</t>
   </si>
   <si>
     <t>Organizations can be corporations, wards, sections, clinical teams, government departments, etc. Note that code is generally a classifier of the type of organization; in many applications, codes are used to identity a particular organization (say, ward) as opposed to another of the same type - these are identifiers, not codes
@@ -679,13 +679,10 @@
     <t>Need to be able to track the kind of organization that this is - different organization types have different uses.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Used to categorize the organization.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/organization-type</t>
+    <t>CARIN RTPBC Pharmacy Type Value Set</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/carin-rtpbc-pharmacy-type</t>
   </si>
   <si>
     <t>No equivalent in v2</t>
@@ -4939,12 +4936,14 @@
       <c r="C31" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" t="s" s="2">
+        <v>207</v>
+      </c>
       <c r="E31" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>40</v>
@@ -4993,13 +4992,13 @@
         <v>40</v>
       </c>
       <c r="W31" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="X31" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="X31" t="s" s="2">
+      <c r="Y31" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>40</v>
@@ -5032,28 +5031,28 @@
         <v>61</v>
       </c>
       <c r="AJ31" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>215</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>123</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E32" t="s" s="2">
         <v>49</v>
@@ -5074,16 +5073,16 @@
         <v>51</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>40</v>
@@ -5132,7 +5131,7 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5147,13 +5146,13 @@
         <v>61</v>
       </c>
       <c r="AJ32" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AK32" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="AK32" t="s" s="2">
+      <c r="AL32" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>40</v>
@@ -5161,7 +5160,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5187,16 +5186,16 @@
         <v>51</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="M33" t="s" s="2">
+      <c r="N33" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>40</v>
@@ -5245,7 +5244,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -5263,7 +5262,7 @@
         <v>40</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>40</v>
@@ -5274,14 +5273,14 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E34" t="s" s="2">
         <v>41</v>
@@ -5299,19 +5298,19 @@
         <v>40</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="K34" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="K34" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="M34" t="s" s="2">
+      <c r="N34" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>235</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>40</v>
@@ -5360,7 +5359,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5369,19 +5368,19 @@
         <v>42</v>
       </c>
       <c r="AH34" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AI34" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="AI34" t="s" s="2">
+      <c r="AJ34" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="AJ34" t="s" s="2">
+      <c r="AK34" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="AK34" t="s" s="2">
+      <c r="AL34" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>40</v>
@@ -5389,7 +5388,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5498,7 +5497,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5609,7 +5608,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5635,10 +5634,10 @@
         <v>69</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5647,7 +5646,7 @@
       </c>
       <c r="P37" s="2"/>
       <c r="Q37" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R37" t="s" s="2">
         <v>40</v>
@@ -5668,49 +5667,49 @@
         <v>134</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Y37" t="s" s="2">
+      <c r="Z37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE37" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="Z37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE37" t="s" s="2">
+      <c r="AF37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH37" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AK37" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="AK37" t="s" s="2">
+      <c r="AL37" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>40</v>
@@ -5718,7 +5717,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5744,16 +5743,16 @@
         <v>51</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5802,7 +5801,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5817,10 +5816,10 @@
         <v>61</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AK38" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>168</v>
@@ -5831,7 +5830,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5857,16 +5856,16 @@
         <v>69</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5894,28 +5893,28 @@
         <v>134</v>
       </c>
       <c r="X39" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="Y39" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="Y39" t="s" s="2">
+      <c r="Z39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE39" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5930,13 +5929,13 @@
         <v>61</v>
       </c>
       <c r="AJ39" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="AK39" t="s" s="2">
+      <c r="AL39" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>40</v>
@@ -5944,7 +5943,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5967,16 +5966,16 @@
         <v>50</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="K40" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="L40" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>277</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
@@ -6026,7 +6025,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -6055,7 +6054,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6081,10 +6080,10 @@
         <v>170</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>281</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6135,7 +6134,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -6153,7 +6152,7 @@
         <v>92</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>176</v>
@@ -6164,14 +6163,14 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E42" t="s" s="2">
         <v>41</v>
@@ -6189,19 +6188,19 @@
         <v>40</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="K42" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="M42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>40</v>
@@ -6250,7 +6249,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6259,19 +6258,19 @@
         <v>42</v>
       </c>
       <c r="AH42" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AI42" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="AI42" t="s" s="2">
+      <c r="AJ42" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="AJ42" t="s" s="2">
+      <c r="AK42" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="AK42" t="s" s="2">
+      <c r="AL42" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>40</v>
@@ -6279,7 +6278,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6388,7 +6387,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6499,7 +6498,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6525,16 +6524,16 @@
         <v>69</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="M45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6547,7 +6546,7 @@
         <v>40</v>
       </c>
       <c r="S45" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T45" t="s" s="2">
         <v>40</v>
@@ -6562,28 +6561,28 @@
         <v>134</v>
       </c>
       <c r="X45" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="Y45" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="Y45" t="s" s="2">
+      <c r="Z45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE45" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="Z45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6598,13 +6597,13 @@
         <v>61</v>
       </c>
       <c r="AJ45" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AL45" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="AK45" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AL45" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>40</v>
@@ -6612,7 +6611,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6638,13 +6637,13 @@
         <v>69</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>311</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6658,7 +6657,7 @@
         <v>40</v>
       </c>
       <c r="S46" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T46" t="s" s="2">
         <v>40</v>
@@ -6673,28 +6672,28 @@
         <v>134</v>
       </c>
       <c r="X46" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="Y46" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="Y46" t="s" s="2">
+      <c r="Z46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE46" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="Z46" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6709,10 +6708,10 @@
         <v>61</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>40</v>
@@ -6723,7 +6722,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6749,16 +6748,16 @@
         <v>51</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="M47" t="s" s="2">
+      <c r="N47" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>40</v>
@@ -6771,43 +6770,43 @@
         <v>40</v>
       </c>
       <c r="S47" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE47" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="T47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6822,10 +6821,10 @@
         <v>61</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AK47" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>40</v>
@@ -6836,7 +6835,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6862,10 +6861,10 @@
         <v>51</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6880,43 +6879,43 @@
         <v>40</v>
       </c>
       <c r="S48" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE48" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="T48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE48" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6931,13 +6930,13 @@
         <v>61</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AK48" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AK48" t="s" s="2">
+      <c r="AL48" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>40</v>
@@ -6945,11 +6944,11 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -6971,10 +6970,10 @@
         <v>51</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6989,43 +6988,43 @@
         <v>40</v>
       </c>
       <c r="S49" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE49" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="T49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -7040,13 +7039,13 @@
         <v>61</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AK49" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AK49" t="s" s="2">
+      <c r="AL49" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AL49" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>40</v>
@@ -7054,11 +7053,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7080,13 +7079,13 @@
         <v>51</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7100,43 +7099,43 @@
         <v>40</v>
       </c>
       <c r="S50" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE50" t="s" s="2">
         <v>348</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>349</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7151,10 +7150,10 @@
         <v>61</v>
       </c>
       <c r="AJ50" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AK50" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
@@ -7165,11 +7164,11 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7191,10 +7190,10 @@
         <v>51</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7224,28 +7223,28 @@
         <v>145</v>
       </c>
       <c r="X51" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="Y51" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="Y51" t="s" s="2">
+      <c r="Z51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE51" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7260,13 +7259,13 @@
         <v>61</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AK51" t="s" s="2">
+      <c r="AL51" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>40</v>
@@ -7274,11 +7273,11 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7300,10 +7299,10 @@
         <v>51</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7318,43 +7317,43 @@
         <v>40</v>
       </c>
       <c r="S52" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE52" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7369,13 +7368,13 @@
         <v>61</v>
       </c>
       <c r="AJ52" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AK52" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="AK52" t="s" s="2">
+      <c r="AL52" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>40</v>
@@ -7383,7 +7382,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7409,13 +7408,13 @@
         <v>51</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7444,28 +7443,28 @@
         <v>134</v>
       </c>
       <c r="X53" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="Y53" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="Y53" t="s" s="2">
+      <c r="Z53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE53" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7480,13 +7479,13 @@
         <v>61</v>
       </c>
       <c r="AJ53" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AK53" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="AK53" t="s" s="2">
+      <c r="AL53" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>40</v>
@@ -7494,7 +7493,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7520,14 +7519,14 @@
         <v>170</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
@@ -7540,43 +7539,43 @@
         <v>40</v>
       </c>
       <c r="S54" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE54" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7591,10 +7590,10 @@
         <v>61</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>176</v>
@@ -7605,7 +7604,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7631,14 +7630,14 @@
         <v>178</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
@@ -7687,7 +7686,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7705,7 +7704,7 @@
         <v>202</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>123</v>
@@ -7716,7 +7715,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7739,19 +7738,19 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>40</v>
@@ -7800,7 +7799,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7818,7 +7817,7 @@
         <v>40</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
@@ -7829,7 +7828,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7938,7 +7937,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8049,11 +8048,11 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -8075,10 +8074,10 @@
         <v>95</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>405</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>98</v>
@@ -8133,7 +8132,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8162,7 +8161,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8188,14 +8187,14 @@
         <v>140</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>40</v>
@@ -8223,11 +8222,11 @@
         <v>145</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>412</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>40</v>
       </c>
@@ -8244,7 +8243,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8262,7 +8261,7 @@
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
@@ -8273,7 +8272,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8296,17 +8295,17 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>40</v>
@@ -8355,7 +8354,7 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8370,10 +8369,10 @@
         <v>61</v>
       </c>
       <c r="AJ61" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="AK61" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>40</v>
@@ -8384,7 +8383,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8407,17 +8406,17 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>40</v>
@@ -8466,7 +8465,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8481,10 +8480,10 @@
         <v>61</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AK62" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
@@ -8495,7 +8494,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8518,17 +8517,17 @@
         <v>40</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>428</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>429</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>40</v>
@@ -8577,7 +8576,7 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -8592,10 +8591,10 @@
         <v>61</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AK63" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
@@ -8606,7 +8605,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8629,17 +8628,17 @@
         <v>40</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>436</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>40</v>
@@ -8688,7 +8687,7 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>

</xml_diff>